<commit_message>
Fix issue with GLO hydrogen market.
</commit_message>
<xml_diff>
--- a/premise/data/additional_inventories/lci-hydrogen-electrolysis.xlsx
+++ b/premise/data/additional_inventories/lci-hydrogen-electrolysis.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10719"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/romain/Github/premise/premise/data/additional_inventories/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/romain/GitHub/premise/premise/data/additional_inventories/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{781D0AD2-CEEE-9E47-8A18-C999A98DF494}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C057B415-CA44-4F49-BBA4-92AFC7BA9ACB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="680" yWindow="1900" windowWidth="29820" windowHeight="24740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="420" yWindow="760" windowWidth="29820" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="lci" sheetId="1" r:id="rId1"/>
@@ -2042,7 +2042,7 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
@@ -2126,10 +2126,22 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2143,21 +2155,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="11" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -2446,8 +2443,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T493"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A451" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A473" sqref="A473:XFD492"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2529,11 +2526,11 @@
       <c r="O5" s="13"/>
       <c r="P5" s="13"/>
     </row>
-    <row r="6" spans="1:20" s="12" customFormat="1" ht="306" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="59" t="s">
+      <c r="B6" s="15" t="s">
         <v>490</v>
       </c>
       <c r="K6" s="13"/>
@@ -15644,10 +15641,10 @@
       <c r="C4" s="39" t="s">
         <v>485</v>
       </c>
-      <c r="D4" s="51" t="s">
+      <c r="D4" s="55" t="s">
         <v>450</v>
       </c>
-      <c r="E4" s="52"/>
+      <c r="E4" s="56"/>
       <c r="F4" s="40" t="s">
         <v>451</v>
       </c>
@@ -15662,10 +15659,10 @@
       <c r="C5" s="39">
         <v>5.5</v>
       </c>
-      <c r="D5" s="53">
+      <c r="D5" s="57">
         <v>2.5</v>
       </c>
-      <c r="E5" s="54"/>
+      <c r="E5" s="58"/>
       <c r="F5" s="39" t="s">
         <v>452</v>
       </c>
@@ -15677,9 +15674,9 @@
       <c r="B6" s="48" t="s">
         <v>454</v>
       </c>
-      <c r="C6" s="49"/>
-      <c r="D6" s="49"/>
-      <c r="E6" s="50"/>
+      <c r="C6" s="54"/>
+      <c r="D6" s="54"/>
+      <c r="E6" s="49"/>
       <c r="F6" s="41" t="s">
         <v>455</v>
       </c>
@@ -15694,10 +15691,10 @@
       <c r="C7" s="39">
         <v>20</v>
       </c>
-      <c r="D7" s="53">
+      <c r="D7" s="57">
         <v>20</v>
       </c>
-      <c r="E7" s="54"/>
+      <c r="E7" s="58"/>
       <c r="F7" s="39" t="s">
         <v>451</v>
       </c>
@@ -15712,10 +15709,10 @@
       <c r="C8" s="39">
         <v>3</v>
       </c>
-      <c r="D8" s="53">
+      <c r="D8" s="57">
         <v>7</v>
       </c>
-      <c r="E8" s="54"/>
+      <c r="E8" s="58"/>
       <c r="F8" s="39" t="s">
         <v>458</v>
       </c>
@@ -15727,9 +15724,9 @@
       <c r="B9" s="48" t="s">
         <v>486</v>
       </c>
-      <c r="C9" s="49"/>
-      <c r="D9" s="49"/>
-      <c r="E9" s="50"/>
+      <c r="C9" s="54"/>
+      <c r="D9" s="54"/>
+      <c r="E9" s="49"/>
       <c r="F9" s="41" t="s">
         <v>460</v>
       </c>
@@ -15801,7 +15798,7 @@
       <c r="D13" s="48">
         <v>23.6</v>
       </c>
-      <c r="E13" s="50"/>
+      <c r="E13" s="49"/>
       <c r="F13" s="39" t="s">
         <v>463</v>
       </c>
@@ -15814,8 +15811,8 @@
         <v>3.7000000000000002E-3</v>
       </c>
       <c r="C14" s="46"/>
-      <c r="D14" s="55"/>
-      <c r="E14" s="56"/>
+      <c r="D14" s="50"/>
+      <c r="E14" s="51"/>
       <c r="F14" s="41" t="s">
         <v>468</v>
       </c>
@@ -15833,7 +15830,7 @@
       <c r="D15" s="48" t="s">
         <v>472</v>
       </c>
-      <c r="E15" s="50"/>
+      <c r="E15" s="49"/>
       <c r="F15" s="39" t="s">
         <v>465</v>
       </c>
@@ -15851,7 +15848,7 @@
       <c r="D16" s="48" t="s">
         <v>476</v>
       </c>
-      <c r="E16" s="50"/>
+      <c r="E16" s="49"/>
       <c r="F16" s="39" t="s">
         <v>451</v>
       </c>
@@ -15866,27 +15863,27 @@
       <c r="C17" s="40" t="s">
         <v>479</v>
       </c>
-      <c r="D17" s="57" t="s">
+      <c r="D17" s="52" t="s">
         <v>480</v>
       </c>
-      <c r="E17" s="58"/>
+      <c r="E17" s="53"/>
       <c r="F17" s="41" t="s">
         <v>481</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="D17:E17"/>
     <mergeCell ref="B9:E9"/>
     <mergeCell ref="D4:E4"/>
     <mergeCell ref="D5:E5"/>
     <mergeCell ref="B6:E6"/>
     <mergeCell ref="D7:E7"/>
     <mergeCell ref="D8:E8"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="D17:E17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Fixes error in electrolyzers dataset: the manufacturing electricity requirements for stacks was three times too high.
</commit_message>
<xml_diff>
--- a/premise/data/additional_inventories/lci-hydrogen-electrolysis.xlsx
+++ b/premise/data/additional_inventories/lci-hydrogen-electrolysis.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11210"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/romain/GitHub/premise/premise/data/additional_inventories/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76C2B965-14EF-8D41-BDD2-7ACC431DD3CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1079E82-ADB6-E644-8098-1A4C6310C3B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35740" yWindow="0" windowWidth="29820" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="lci" sheetId="1" r:id="rId1"/>
@@ -2152,22 +2152,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2181,6 +2169,18 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -2469,8 +2469,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T499"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView topLeftCell="A192" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B217" sqref="B217"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3702,7 +3702,7 @@
         <v>35</v>
       </c>
       <c r="B46" s="13">
-        <v>311672</v>
+        <v>103890.7681</v>
       </c>
       <c r="C46" s="12" t="s">
         <v>18</v>
@@ -8356,7 +8356,7 @@
         <v>35</v>
       </c>
       <c r="B222" s="13">
-        <v>286659.90000000002</v>
+        <v>95553.31568</v>
       </c>
       <c r="C222" s="12" t="s">
         <v>18</v>
@@ -13104,7 +13104,7 @@
         <v>35</v>
       </c>
       <c r="B392" s="13">
-        <v>366673.3</v>
+        <v>122224.433</v>
       </c>
       <c r="C392" s="12" t="s">
         <v>18</v>
@@ -16122,8 +16122,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D607540C-5A98-C943-82C9-9BA357D77C9A}">
   <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -16169,10 +16169,10 @@
       <c r="C4" s="39" t="s">
         <v>484</v>
       </c>
-      <c r="D4" s="57" t="s">
+      <c r="D4" s="53" t="s">
         <v>449</v>
       </c>
-      <c r="E4" s="58"/>
+      <c r="E4" s="54"/>
       <c r="F4" s="40" t="s">
         <v>450</v>
       </c>
@@ -16187,10 +16187,10 @@
       <c r="C5" s="39">
         <v>5.5</v>
       </c>
-      <c r="D5" s="59">
+      <c r="D5" s="55">
         <v>2.5</v>
       </c>
-      <c r="E5" s="60"/>
+      <c r="E5" s="56"/>
       <c r="F5" s="39" t="s">
         <v>451</v>
       </c>
@@ -16202,9 +16202,9 @@
       <c r="B6" s="50" t="s">
         <v>453</v>
       </c>
-      <c r="C6" s="56"/>
-      <c r="D6" s="56"/>
-      <c r="E6" s="51"/>
+      <c r="C6" s="51"/>
+      <c r="D6" s="51"/>
+      <c r="E6" s="52"/>
       <c r="F6" s="41" t="s">
         <v>454</v>
       </c>
@@ -16219,10 +16219,10 @@
       <c r="C7" s="39">
         <v>20</v>
       </c>
-      <c r="D7" s="59">
+      <c r="D7" s="55">
         <v>20</v>
       </c>
-      <c r="E7" s="60"/>
+      <c r="E7" s="56"/>
       <c r="F7" s="39" t="s">
         <v>450</v>
       </c>
@@ -16237,10 +16237,10 @@
       <c r="C8" s="39">
         <v>3</v>
       </c>
-      <c r="D8" s="59">
+      <c r="D8" s="55">
         <v>7</v>
       </c>
-      <c r="E8" s="60"/>
+      <c r="E8" s="56"/>
       <c r="F8" s="39" t="s">
         <v>457</v>
       </c>
@@ -16252,9 +16252,9 @@
       <c r="B9" s="50" t="s">
         <v>485</v>
       </c>
-      <c r="C9" s="56"/>
-      <c r="D9" s="56"/>
-      <c r="E9" s="51"/>
+      <c r="C9" s="51"/>
+      <c r="D9" s="51"/>
+      <c r="E9" s="52"/>
       <c r="F9" s="41" t="s">
         <v>459</v>
       </c>
@@ -16326,7 +16326,7 @@
       <c r="D13" s="50">
         <v>23.6</v>
       </c>
-      <c r="E13" s="51"/>
+      <c r="E13" s="52"/>
       <c r="F13" s="39" t="s">
         <v>462</v>
       </c>
@@ -16339,8 +16339,8 @@
         <v>3.7000000000000002E-3</v>
       </c>
       <c r="C14" s="46"/>
-      <c r="D14" s="52"/>
-      <c r="E14" s="53"/>
+      <c r="D14" s="57"/>
+      <c r="E14" s="58"/>
       <c r="F14" s="41" t="s">
         <v>467</v>
       </c>
@@ -16358,7 +16358,7 @@
       <c r="D15" s="50" t="s">
         <v>471</v>
       </c>
-      <c r="E15" s="51"/>
+      <c r="E15" s="52"/>
       <c r="F15" s="39" t="s">
         <v>464</v>
       </c>
@@ -16376,7 +16376,7 @@
       <c r="D16" s="50" t="s">
         <v>475</v>
       </c>
-      <c r="E16" s="51"/>
+      <c r="E16" s="52"/>
       <c r="F16" s="39" t="s">
         <v>450</v>
       </c>
@@ -16391,27 +16391,27 @@
       <c r="C17" s="40" t="s">
         <v>478</v>
       </c>
-      <c r="D17" s="54" t="s">
+      <c r="D17" s="59" t="s">
         <v>479</v>
       </c>
-      <c r="E17" s="55"/>
+      <c r="E17" s="60"/>
       <c r="F17" s="41" t="s">
         <v>480</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="D17:E17"/>
     <mergeCell ref="B9:E9"/>
     <mergeCell ref="D4:E4"/>
     <mergeCell ref="D5:E5"/>
     <mergeCell ref="B6:E6"/>
     <mergeCell ref="D7:E7"/>
     <mergeCell ref="D8:E8"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="D17:E17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Fixed issue with electrolyzers' stack EoL treatments
</commit_message>
<xml_diff>
--- a/premise/data/additional_inventories/lci-hydrogen-electrolysis.xlsx
+++ b/premise/data/additional_inventories/lci-hydrogen-electrolysis.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10817"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/romain/GitHub/premise/premise/data/additional_inventories/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/romain/Github/premise/premise/data/additional_inventories/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E0046B9-DD95-1040-8051-A7A40AA5EE13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C63BB10-A47E-6444-8FAC-93041FEF97A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2211,22 +2211,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2241,6 +2229,18 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Neutral" xfId="4" builtinId="28"/>
@@ -2248,7 +2248,7 @@
     <cellStyle name="Normal 11 3" xfId="1" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
     <cellStyle name="Normal 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
     <cellStyle name="Normal 3" xfId="3" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
-    <cellStyle name="Per cent" xfId="5" builtinId="5"/>
+    <cellStyle name="Percent" xfId="5" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2528,8 +2528,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U589"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+    <sheetView tabSelected="1" topLeftCell="A422" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B460" sqref="B460"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -11318,7 +11318,8 @@
         <v>204</v>
       </c>
       <c r="B289" s="11">
-        <v>-60583</v>
+        <f>-1*B274</f>
+        <v>-20194.400000000001</v>
       </c>
       <c r="C289" s="11" t="s">
         <v>37</v>
@@ -11347,7 +11348,8 @@
         <v>210</v>
       </c>
       <c r="B290" s="11">
-        <v>-579</v>
+        <f>-1*SUM(B272,B276)</f>
+        <v>-193</v>
       </c>
       <c r="C290" s="11" t="s">
         <v>212</v>
@@ -16193,7 +16195,8 @@
         <v>204</v>
       </c>
       <c r="B459" s="11">
-        <v>-26928</v>
+        <f>-1*B434</f>
+        <v>-8976.1</v>
       </c>
       <c r="C459" s="11" t="s">
         <v>37</v>
@@ -19850,10 +19853,10 @@
       <c r="C4" s="38" t="s">
         <v>430</v>
       </c>
-      <c r="D4" s="56" t="s">
+      <c r="D4" s="52" t="s">
         <v>395</v>
       </c>
-      <c r="E4" s="57"/>
+      <c r="E4" s="53"/>
       <c r="F4" s="39" t="s">
         <v>396</v>
       </c>
@@ -19868,10 +19871,10 @@
       <c r="C5" s="38">
         <v>5.5</v>
       </c>
-      <c r="D5" s="58">
+      <c r="D5" s="54">
         <v>2.5</v>
       </c>
-      <c r="E5" s="59"/>
+      <c r="E5" s="55"/>
       <c r="F5" s="38" t="s">
         <v>397</v>
       </c>
@@ -19883,9 +19886,9 @@
       <c r="B6" s="49" t="s">
         <v>399</v>
       </c>
-      <c r="C6" s="55"/>
-      <c r="D6" s="55"/>
-      <c r="E6" s="50"/>
+      <c r="C6" s="50"/>
+      <c r="D6" s="50"/>
+      <c r="E6" s="51"/>
       <c r="F6" s="40" t="s">
         <v>400</v>
       </c>
@@ -19900,10 +19903,10 @@
       <c r="C7" s="38">
         <v>20</v>
       </c>
-      <c r="D7" s="58">
+      <c r="D7" s="54">
         <v>20</v>
       </c>
-      <c r="E7" s="59"/>
+      <c r="E7" s="55"/>
       <c r="F7" s="38" t="s">
         <v>396</v>
       </c>
@@ -19918,10 +19921,10 @@
       <c r="C8" s="38">
         <v>3</v>
       </c>
-      <c r="D8" s="58">
+      <c r="D8" s="54">
         <v>7</v>
       </c>
-      <c r="E8" s="59"/>
+      <c r="E8" s="55"/>
       <c r="F8" s="38" t="s">
         <v>403</v>
       </c>
@@ -19933,9 +19936,9 @@
       <c r="B9" s="49" t="s">
         <v>431</v>
       </c>
-      <c r="C9" s="55"/>
-      <c r="D9" s="55"/>
-      <c r="E9" s="50"/>
+      <c r="C9" s="50"/>
+      <c r="D9" s="50"/>
+      <c r="E9" s="51"/>
       <c r="F9" s="40" t="s">
         <v>405</v>
       </c>
@@ -20007,7 +20010,7 @@
       <c r="D13" s="49">
         <v>23.6</v>
       </c>
-      <c r="E13" s="50"/>
+      <c r="E13" s="51"/>
       <c r="F13" s="38" t="s">
         <v>408</v>
       </c>
@@ -20020,8 +20023,8 @@
         <v>3.7000000000000002E-3</v>
       </c>
       <c r="C14" s="45"/>
-      <c r="D14" s="51"/>
-      <c r="E14" s="52"/>
+      <c r="D14" s="56"/>
+      <c r="E14" s="57"/>
       <c r="F14" s="40" t="s">
         <v>413</v>
       </c>
@@ -20039,7 +20042,7 @@
       <c r="D15" s="49" t="s">
         <v>417</v>
       </c>
-      <c r="E15" s="50"/>
+      <c r="E15" s="51"/>
       <c r="F15" s="38" t="s">
         <v>410</v>
       </c>
@@ -20057,7 +20060,7 @@
       <c r="D16" s="49" t="s">
         <v>421</v>
       </c>
-      <c r="E16" s="50"/>
+      <c r="E16" s="51"/>
       <c r="F16" s="38" t="s">
         <v>396</v>
       </c>
@@ -20072,27 +20075,27 @@
       <c r="C17" s="39" t="s">
         <v>424</v>
       </c>
-      <c r="D17" s="53" t="s">
+      <c r="D17" s="58" t="s">
         <v>425</v>
       </c>
-      <c r="E17" s="54"/>
+      <c r="E17" s="59"/>
       <c r="F17" s="40" t="s">
         <v>426</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="D17:E17"/>
     <mergeCell ref="B9:E9"/>
     <mergeCell ref="D4:E4"/>
     <mergeCell ref="D5:E5"/>
     <mergeCell ref="B6:E6"/>
     <mergeCell ref="D7:E7"/>
     <mergeCell ref="D8:E8"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="D17:E17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Fix deionized water inventories Fix datapackage exports Fix the identification of fuels
</commit_message>
<xml_diff>
--- a/premise/data/additional_inventories/lci-hydrogen-electrolysis.xlsx
+++ b/premise/data/additional_inventories/lci-hydrogen-electrolysis.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/romain/Github/premise/premise/data/additional_inventories/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/romain/GitHub/premise/premise/data/additional_inventories/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C63BB10-A47E-6444-8FAC-93041FEF97A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57D8C29F-CA9A-4C42-A35D-878E671CD9FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="34920" yWindow="760" windowWidth="25800" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="lci" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="Manufacturers' data" sheetId="2" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">lci!$A$1:$T$597</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">lci!$A$1:$T$598</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Manufacturers'' data'!$A$3:$AG$104</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3318" uniqueCount="542">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3340" uniqueCount="546">
   <si>
     <t>Database</t>
   </si>
@@ -1821,44 +1821,54 @@
     <t>Depends on salinity. 1.4-1.7 kWh/m3 of brackish water, with miximum posisble values up to 2.5 kWh.</t>
   </si>
   <si>
+    <t>3.6-5.7 kWh/m3 of sea water.</t>
+  </si>
+  <si>
+    <t>1 kg of demineralized and deionized water, from sea water. Adapted from inventories from the following report: LIFE CYCLE ASSESSMENT OF HYDROGEN PRODUCTION PATHWAYS IN CANADA, Giovanna Gonzales-Calienes et al., 2022. https://publications.gc.ca/collections/collection_2022/cnrc-nrc/NR16-399-2022-eng.pdf, but electricity conusmption has been adapted to represent the treatment of high salinity water, based on ﻿Hausmann, J. N., Schlögl, R., Menezes, P. W., &amp; Driess, M. (2021). Is direct seawater splitting economically meaningful? Energy and Environmental Science, 14(7), 3679–3685. https://doi.org/10.1039/d0ee03659e.</t>
+  </si>
+  <si>
+    <t>Water, salt, ocean</t>
+  </si>
+  <si>
+    <t>Recovery rate of 40% for seawater.</t>
+  </si>
+  <si>
+    <t>Water</t>
+  </si>
+  <si>
+    <t>water</t>
+  </si>
+  <si>
+    <t>Brine release</t>
+  </si>
+  <si>
+    <t>market for acrylic dispersion, with water, in 58% solution</t>
+  </si>
+  <si>
+    <t>Chlorine</t>
+  </si>
+  <si>
+    <t>5.2 mg Chlorine (as Cl2)/liter brine.</t>
+  </si>
+  <si>
+    <t>Sodium hydroxide</t>
+  </si>
+  <si>
+    <t>1.7 mg Sodium hydroxide (as NaOH)/liter brine.</t>
+  </si>
+  <si>
+    <t>Sulfuric acid</t>
+  </si>
+  <si>
+    <t>31 mg Sulfuric acid (as H2SO4)/liter brine.</t>
+  </si>
+  <si>
     <t>1 kg of demineralized and deionized water. Inventories from the following report: Life Cycle Assessment of Hydrogen production pathways in Canada, Giovanna Gonzales-Calienes et al., 2022. 
 https://publications.gc.ca/collections/collection_2022/cnrc-nrc/NR16-399-2022-eng.pdf
-Description from the report: "The reverse osmosis process was used since it is one of the most common desalination technologies. The energy requirement is highly dependent on the water quality (such as
-salinity) of the available source since it mainly comes from the use of high-pressure pumps. The quality of feed water is location-dependent for the real plant. In our study, the plant is assumed to be near a river or
-lake for easy access to fresh water and brine discharge, and hence the water is assumed to be brackish water (salinity of 1-15 g/L), and a brackish water RO (BWRO) rather than the seawater RO is considered.
+Description from the report: "The reverse osmosis process was used since it is one of the most common desalination technologies. The energy requirement is highly dependent on the water quality (such as salinity) of the available source since it mainly comes from the use of high-pressure pumps. The quality of feed water is location-dependent for the real plant. In our study, the plant is assumed to be near a river or lake for easy access to fresh water and brine discharge, and hence the water is assumed to be brackish water (salinity of 1-15 g/L), and a brackish water RO (BWRO) rather than the seawater RO is considered.
 The recovery ratio of the water (flow rate ratio of generated clean water to the brackish feed water) by BWRO can range from 50% to 90%, depending on the different configurations adopted (Pan et al., 2020).
-The average water recovery ratio of 70% was assumed. The energy consumption to produce a unit of deionized water generally can vary from 0.8-2.5 kWh/m3 based on the review of BWRO plants (Pan et al.,
-2020). A specific energy requirement of 1.55 kWh/m3 is assumed for the RO in this AE plant, which is an average value of 1.4-1.7 kWh/m3 from a RO process with treatment capacity of 360 m3/day (Pan et al., 2020)."</t>
-  </si>
-  <si>
-    <t>3.6-5.7 kWh/m3 of sea water.</t>
-  </si>
-  <si>
-    <t>1 kg of demineralized and deionized water, from sea water. Adapted from inventories from the following report: LIFE CYCLE ASSESSMENT OF HYDROGEN PRODUCTION PATHWAYS IN CANADA, Giovanna Gonzales-Calienes et al., 2022. https://publications.gc.ca/collections/collection_2022/cnrc-nrc/NR16-399-2022-eng.pdf, but electricity conusmption has been adapted to represent the treatment of high salinity water, based on ﻿Hausmann, J. N., Schlögl, R., Menezes, P. W., &amp; Driess, M. (2021). Is direct seawater splitting economically meaningful? Energy and Environmental Science, 14(7), 3679–3685. https://doi.org/10.1039/d0ee03659e.</t>
-  </si>
-  <si>
-    <t>Water, salt, ocean</t>
-  </si>
-  <si>
-    <t>Recovery rate of 40% for seawater.</t>
-  </si>
-  <si>
-    <t>Water</t>
-  </si>
-  <si>
-    <t>water</t>
-  </si>
-  <si>
-    <t>Brine release</t>
-  </si>
-  <si>
-    <t>Sodium I</t>
-  </si>
-  <si>
-    <t>Chloride</t>
-  </si>
-  <si>
-    <t>market for acrylic dispersion, with water, in 58% solution</t>
+The average water recovery ratio of 70% was assumed. The energy consumption to produce a unit of deionized water generally can vary from 0.8-2.5 kWh/m3 based on the review of BWRO plants (Pan et al., 2020). A specific energy requirement of 1.55 kWh/m3 is assumed for the RO in this AE plant, which is an average value of 1.4-1.7 kWh/m3 from a RO process with treatment capacity of 360 m3/day (Pan et al., 2020)."
+Note: we could not represent the emissions of dissolved salts (~33g/L) and antiscalant (~7mg/L) to water.</t>
   </si>
 </sst>
 </file>
@@ -2211,10 +2221,22 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2229,18 +2251,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Neutral" xfId="4" builtinId="28"/>
@@ -2248,7 +2258,7 @@
     <cellStyle name="Normal 11 3" xfId="1" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
     <cellStyle name="Normal 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
     <cellStyle name="Normal 3" xfId="3" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
-    <cellStyle name="Percent" xfId="5" builtinId="5"/>
+    <cellStyle name="Per cent" xfId="5" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2526,10 +2536,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U589"/>
+  <dimension ref="A1:U593"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A422" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B460" sqref="B460"/>
+    <sheetView tabSelected="1" topLeftCell="A571" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B594" sqref="B594"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -19023,7 +19033,7 @@
         <v>11</v>
       </c>
       <c r="B558" s="14" t="s">
-        <v>531</v>
+        <v>545</v>
       </c>
       <c r="K558" s="12"/>
       <c r="L558" s="12"/>
@@ -19307,7 +19317,7 @@
     </row>
     <row r="569" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A569" t="s">
-        <v>541</v>
+        <v>538</v>
       </c>
       <c r="B569" s="4">
         <v>2.7E-6</v>
@@ -19366,7 +19376,7 @@
     </row>
     <row r="571" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A571" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="B571" s="4">
         <f>B570-(1/1000)</f>
@@ -19376,13 +19386,16 @@
         <v>31</v>
       </c>
       <c r="E571" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="F571" t="s">
         <v>14</v>
       </c>
       <c r="H571" t="s">
-        <v>538</v>
+        <v>537</v>
+      </c>
+      <c r="I571">
+        <v>0</v>
       </c>
     </row>
     <row r="572" spans="1:21" x14ac:dyDescent="0.2">
@@ -19390,57 +19403,81 @@
         <v>539</v>
       </c>
       <c r="B572" s="4">
-        <v>4.5799999999999999E-3</v>
+        <f>(5.2/0.000001)*(B571*1000)</f>
+        <v>2228571.4285714286</v>
       </c>
       <c r="D572" t="s">
         <v>13</v>
       </c>
       <c r="E572" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="F572" t="s">
         <v>14</v>
       </c>
+      <c r="H572" t="s">
+        <v>540</v>
+      </c>
+      <c r="I572">
+        <v>0</v>
+      </c>
     </row>
     <row r="573" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A573" t="s">
-        <v>540</v>
+        <v>541</v>
       </c>
       <c r="B573" s="4">
-        <v>6.8599999999999998E-3</v>
+        <f>(1.7/0.000001)*(B571*1000)</f>
+        <v>728571.42857142852</v>
       </c>
       <c r="D573" t="s">
         <v>13</v>
       </c>
       <c r="E573" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="F573" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="575" spans="1:21" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A575" s="8" t="s">
+      <c r="H573" t="s">
+        <v>542</v>
+      </c>
+      <c r="I573">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="574" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A574" t="s">
+        <v>543</v>
+      </c>
+      <c r="B574" s="4">
+        <f>(31/0.000001)*(B571*1000)</f>
+        <v>13285714.285714285</v>
+      </c>
+      <c r="D574" t="s">
+        <v>13</v>
+      </c>
+      <c r="E574" t="s">
+        <v>536</v>
+      </c>
+      <c r="F574" t="s">
+        <v>14</v>
+      </c>
+      <c r="H574" t="s">
+        <v>544</v>
+      </c>
+      <c r="I574">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="576" spans="1:21" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A576" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B575" s="9" t="s">
+      <c r="B576" s="9" t="s">
         <v>529</v>
       </c>
-      <c r="C575" s="10"/>
-      <c r="K575" s="12"/>
-      <c r="L575" s="12"/>
-      <c r="M575" s="12"/>
-      <c r="N575" s="12"/>
-      <c r="O575" s="12"/>
-      <c r="P575" s="12"/>
-    </row>
-    <row r="576" spans="1:21" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A576" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="B576" s="14">
-        <v>1</v>
-      </c>
+      <c r="C576" s="10"/>
       <c r="K576" s="12"/>
       <c r="L576" s="12"/>
       <c r="M576" s="12"/>
@@ -19450,10 +19487,10 @@
     </row>
     <row r="577" spans="1:21" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A577" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="B577" s="14" t="s">
-        <v>533</v>
+        <v>3</v>
+      </c>
+      <c r="B577" s="14">
+        <v>1</v>
       </c>
       <c r="K577" s="12"/>
       <c r="L577" s="12"/>
@@ -19464,10 +19501,10 @@
     </row>
     <row r="578" spans="1:21" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A578" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="B578" s="15" t="s">
-        <v>518</v>
+        <v>11</v>
+      </c>
+      <c r="B578" s="14" t="s">
+        <v>532</v>
       </c>
       <c r="K578" s="12"/>
       <c r="L578" s="12"/>
@@ -19478,10 +19515,10 @@
     </row>
     <row r="579" spans="1:21" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A579" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="B579" s="14" t="s">
-        <v>34</v>
+        <v>4</v>
+      </c>
+      <c r="B579" s="15" t="s">
+        <v>518</v>
       </c>
       <c r="K579" s="12"/>
       <c r="L579" s="12"/>
@@ -19492,14 +19529,11 @@
     </row>
     <row r="580" spans="1:21" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A580" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="B580" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="H580" s="17"/>
-      <c r="I580" s="17"/>
-      <c r="J580" s="17"/>
+        <v>2</v>
+      </c>
+      <c r="B580" s="14" t="s">
+        <v>34</v>
+      </c>
       <c r="K580" s="12"/>
       <c r="L580" s="12"/>
       <c r="M580" s="12"/>
@@ -19508,18 +19542,15 @@
       <c r="P580" s="12"/>
     </row>
     <row r="581" spans="1:21" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A581" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="B581" s="9"/>
-      <c r="C581" s="17"/>
-      <c r="D581" s="17"/>
-      <c r="E581" s="17"/>
-      <c r="F581" s="17"/>
-      <c r="G581" s="17"/>
-      <c r="H581" s="10"/>
-      <c r="I581" s="10"/>
-      <c r="J581" s="10"/>
+      <c r="A581" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B581" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="H581" s="17"/>
+      <c r="I581" s="17"/>
+      <c r="J581" s="17"/>
       <c r="K581" s="12"/>
       <c r="L581" s="12"/>
       <c r="M581" s="12"/>
@@ -19529,176 +19560,173 @@
     </row>
     <row r="582" spans="1:21" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A582" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="B582" s="9"/>
+      <c r="C582" s="17"/>
+      <c r="D582" s="17"/>
+      <c r="E582" s="17"/>
+      <c r="F582" s="17"/>
+      <c r="G582" s="17"/>
+      <c r="H582" s="10"/>
+      <c r="I582" s="10"/>
+      <c r="J582" s="10"/>
+      <c r="K582" s="12"/>
+      <c r="L582" s="12"/>
+      <c r="M582" s="12"/>
+      <c r="N582" s="12"/>
+      <c r="O582" s="12"/>
+      <c r="P582" s="12"/>
+    </row>
+    <row r="583" spans="1:21" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A583" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="B582" s="17" t="s">
+      <c r="B583" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="C582" s="17" t="s">
+      <c r="C583" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="D582" s="17" t="s">
+      <c r="D583" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="E582" s="17" t="s">
+      <c r="E583" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="F582" s="17" t="s">
+      <c r="F583" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="G582" s="17" t="s">
+      <c r="G583" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="H582" s="17" t="s">
+      <c r="H583" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="I582" s="17" t="s">
+      <c r="I583" s="17" t="s">
         <v>466</v>
       </c>
-      <c r="J582" s="7" t="s">
+      <c r="J583" s="7" t="s">
         <v>467</v>
       </c>
-      <c r="K582" s="18" t="s">
+      <c r="K583" s="18" t="s">
         <v>468</v>
       </c>
-      <c r="L582" s="18" t="s">
+      <c r="L583" s="18" t="s">
         <v>469</v>
       </c>
-      <c r="M582" s="18" t="s">
+      <c r="M583" s="18" t="s">
         <v>470</v>
       </c>
-      <c r="N582" s="18" t="s">
+      <c r="N583" s="18" t="s">
         <v>471</v>
       </c>
-      <c r="O582" s="18" t="s">
+      <c r="O583" s="18" t="s">
         <v>472</v>
       </c>
-      <c r="P582" s="18" t="s">
+      <c r="P583" s="18" t="s">
         <v>473</v>
       </c>
-      <c r="Q582" s="7" t="s">
+      <c r="Q583" s="7" t="s">
         <v>474</v>
       </c>
-      <c r="R582" s="7" t="s">
+      <c r="R583" s="7" t="s">
         <v>475</v>
       </c>
-      <c r="S582" s="17" t="s">
+      <c r="S583" s="17" t="s">
         <v>476</v>
       </c>
-      <c r="T582" s="7" t="s">
+      <c r="T583" s="7" t="s">
         <v>477</v>
       </c>
-      <c r="U582" s="17" t="s">
+      <c r="U583" s="17" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="583" spans="1:21" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A583" s="16" t="str">
-        <f>B575</f>
+    <row r="584" spans="1:21" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A584" s="16" t="str">
+        <f>B576</f>
         <v>deionized water production, via reverse osmosis, from sea water</v>
       </c>
-      <c r="B583" s="16">
+      <c r="B584" s="16">
         <v>1</v>
       </c>
-      <c r="C583" s="11" t="str">
+      <c r="C584" s="11" t="str">
+        <f>B580</f>
+        <v>RER</v>
+      </c>
+      <c r="D584" s="11" t="str">
+        <f>B581</f>
+        <v>kilogram</v>
+      </c>
+      <c r="E584" s="10"/>
+      <c r="F584" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="G584" s="16" t="str">
         <f>B579</f>
-        <v>RER</v>
-      </c>
-      <c r="D583" s="11" t="str">
-        <f>B580</f>
-        <v>kilogram</v>
-      </c>
-      <c r="E583" s="10"/>
-      <c r="F583" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="G583" s="16" t="str">
-        <f>B578</f>
         <v>water, deionized</v>
       </c>
-      <c r="H583" s="10"/>
-      <c r="I583" s="10">
+      <c r="H584" s="10"/>
+      <c r="I584" s="10">
         <v>0</v>
       </c>
-      <c r="K583" s="12"/>
-      <c r="L583" s="12"/>
-      <c r="M583" s="12"/>
-      <c r="N583" s="12"/>
-      <c r="O583" s="12"/>
-      <c r="P583" s="12"/>
-      <c r="T583"/>
-    </row>
-    <row r="584" spans="1:21" ht="16" x14ac:dyDescent="0.2">
-      <c r="A584" t="s">
+      <c r="K584" s="12"/>
+      <c r="L584" s="12"/>
+      <c r="M584" s="12"/>
+      <c r="N584" s="12"/>
+      <c r="O584" s="12"/>
+      <c r="P584" s="12"/>
+      <c r="T584"/>
+    </row>
+    <row r="585" spans="1:21" ht="16" x14ac:dyDescent="0.2">
+      <c r="A585" t="s">
         <v>33</v>
       </c>
-      <c r="B584" s="4">
+      <c r="B585" s="4">
         <f>AVERAGE(3.6, 5.7)/1000</f>
         <v>4.6500000000000005E-3</v>
       </c>
-      <c r="C584" s="11" t="s">
+      <c r="C585" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="D584" t="s">
+      <c r="D585" t="s">
         <v>35</v>
       </c>
-      <c r="F584" t="s">
-        <v>12</v>
-      </c>
-      <c r="G584" t="s">
+      <c r="F585" t="s">
+        <v>12</v>
+      </c>
+      <c r="G585" t="s">
         <v>36</v>
       </c>
-      <c r="H584" t="s">
-        <v>532</v>
-      </c>
-      <c r="I584">
+      <c r="H585" t="s">
+        <v>531</v>
+      </c>
+      <c r="I585">
         <v>5</v>
       </c>
-      <c r="J584" s="4">
-        <f>B584</f>
+      <c r="J585" s="4">
+        <f>B585</f>
         <v>4.6500000000000005E-3</v>
       </c>
-      <c r="S584">
+      <c r="S585">
         <f>3.6/1000</f>
         <v>3.5999999999999999E-3</v>
       </c>
-      <c r="T584">
+      <c r="T585">
         <f>5.7/1000</f>
         <v>5.7000000000000002E-3</v>
       </c>
     </row>
-    <row r="585" spans="1:21" ht="16" x14ac:dyDescent="0.2">
-      <c r="A585" t="s">
-        <v>519</v>
-      </c>
-      <c r="B585" s="4">
-        <v>1.3499999999999999E-5</v>
-      </c>
-      <c r="C585" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="D585" t="s">
-        <v>13</v>
-      </c>
-      <c r="F585" t="s">
-        <v>12</v>
-      </c>
-      <c r="G585" t="s">
-        <v>520</v>
-      </c>
-      <c r="I585">
-        <v>0</v>
-      </c>
-    </row>
     <row r="586" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A586" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="B586" s="4">
-        <v>7.5799999999999998E-7</v>
+        <v>1.3499999999999999E-5</v>
       </c>
       <c r="C586" s="11" t="s">
-        <v>17</v>
+        <v>34</v>
       </c>
       <c r="D586" t="s">
         <v>13</v>
@@ -19707,7 +19735,7 @@
         <v>12</v>
       </c>
       <c r="G586" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="I586">
         <v>0</v>
@@ -19715,13 +19743,13 @@
     </row>
     <row r="587" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A587" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="B587" s="4">
-        <v>2.1600000000000001E-6</v>
+        <v>7.5799999999999998E-7</v>
       </c>
       <c r="C587" s="11" t="s">
-        <v>34</v>
+        <v>17</v>
       </c>
       <c r="D587" t="s">
         <v>13</v>
@@ -19730,7 +19758,7 @@
         <v>12</v>
       </c>
       <c r="G587" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="I587">
         <v>0</v>
@@ -19738,10 +19766,10 @@
     </row>
     <row r="588" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A588" t="s">
-        <v>541</v>
+        <v>523</v>
       </c>
       <c r="B588" s="4">
-        <v>2.7E-6</v>
+        <v>2.1600000000000001E-6</v>
       </c>
       <c r="C588" s="11" t="s">
         <v>34</v>
@@ -19753,50 +19781,145 @@
         <v>12</v>
       </c>
       <c r="G588" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="I588">
         <v>0</v>
       </c>
     </row>
-    <row r="589" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="589" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A589" t="s">
-        <v>534</v>
+        <v>538</v>
       </c>
       <c r="B589" s="4">
+        <v>2.7E-6</v>
+      </c>
+      <c r="C589" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="D589" t="s">
+        <v>13</v>
+      </c>
+      <c r="F589" t="s">
+        <v>12</v>
+      </c>
+      <c r="G589" t="s">
+        <v>525</v>
+      </c>
+      <c r="I589">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="590" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A590" t="s">
+        <v>533</v>
+      </c>
+      <c r="B590" s="4">
         <f>1/0.4/1000</f>
         <v>2.5000000000000001E-3</v>
       </c>
-      <c r="D589" t="s">
+      <c r="D590" t="s">
         <v>31</v>
       </c>
-      <c r="E589" t="s">
+      <c r="E590" t="s">
         <v>527</v>
       </c>
-      <c r="F589" t="s">
+      <c r="F590" t="s">
         <v>14</v>
       </c>
-      <c r="H589" t="s">
-        <v>535</v>
-      </c>
-      <c r="I589">
+      <c r="H590" t="s">
+        <v>534</v>
+      </c>
+      <c r="I590">
         <v>5</v>
       </c>
-      <c r="J589" s="4">
-        <f>B589</f>
+      <c r="J590" s="4">
+        <f>B590</f>
         <v>2.5000000000000001E-3</v>
       </c>
-      <c r="S589" s="4">
+      <c r="S590" s="4">
         <f>1/0.5/1000</f>
         <v>2E-3</v>
       </c>
-      <c r="T589" s="4">
+      <c r="T590" s="4">
         <f>1/0.35/1000</f>
         <v>2.8571428571428571E-3</v>
       </c>
     </row>
+    <row r="591" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A591" t="s">
+        <v>539</v>
+      </c>
+      <c r="B591" s="4">
+        <f>(5.2/0.000001)*(B590*1000)</f>
+        <v>13000000</v>
+      </c>
+      <c r="D591" t="s">
+        <v>13</v>
+      </c>
+      <c r="E591" t="s">
+        <v>536</v>
+      </c>
+      <c r="F591" t="s">
+        <v>14</v>
+      </c>
+      <c r="H591" t="s">
+        <v>540</v>
+      </c>
+      <c r="I591">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="592" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A592" t="s">
+        <v>541</v>
+      </c>
+      <c r="B592" s="4">
+        <f>(1.7/0.000001)*(B590*1000)</f>
+        <v>4250000</v>
+      </c>
+      <c r="D592" t="s">
+        <v>13</v>
+      </c>
+      <c r="E592" t="s">
+        <v>536</v>
+      </c>
+      <c r="F592" t="s">
+        <v>14</v>
+      </c>
+      <c r="H592" t="s">
+        <v>542</v>
+      </c>
+      <c r="I592">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="593" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A593" t="s">
+        <v>543</v>
+      </c>
+      <c r="B593" s="4">
+        <f>(31/0.000001)*(B590*1000)</f>
+        <v>77500000</v>
+      </c>
+      <c r="D593" t="s">
+        <v>13</v>
+      </c>
+      <c r="E593" t="s">
+        <v>536</v>
+      </c>
+      <c r="F593" t="s">
+        <v>14</v>
+      </c>
+      <c r="H593" t="s">
+        <v>544</v>
+      </c>
+      <c r="I593">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:T597" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:T598" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -19853,10 +19976,10 @@
       <c r="C4" s="38" t="s">
         <v>430</v>
       </c>
-      <c r="D4" s="52" t="s">
+      <c r="D4" s="56" t="s">
         <v>395</v>
       </c>
-      <c r="E4" s="53"/>
+      <c r="E4" s="57"/>
       <c r="F4" s="39" t="s">
         <v>396</v>
       </c>
@@ -19871,10 +19994,10 @@
       <c r="C5" s="38">
         <v>5.5</v>
       </c>
-      <c r="D5" s="54">
+      <c r="D5" s="58">
         <v>2.5</v>
       </c>
-      <c r="E5" s="55"/>
+      <c r="E5" s="59"/>
       <c r="F5" s="38" t="s">
         <v>397</v>
       </c>
@@ -19886,9 +20009,9 @@
       <c r="B6" s="49" t="s">
         <v>399</v>
       </c>
-      <c r="C6" s="50"/>
-      <c r="D6" s="50"/>
-      <c r="E6" s="51"/>
+      <c r="C6" s="55"/>
+      <c r="D6" s="55"/>
+      <c r="E6" s="50"/>
       <c r="F6" s="40" t="s">
         <v>400</v>
       </c>
@@ -19903,10 +20026,10 @@
       <c r="C7" s="38">
         <v>20</v>
       </c>
-      <c r="D7" s="54">
+      <c r="D7" s="58">
         <v>20</v>
       </c>
-      <c r="E7" s="55"/>
+      <c r="E7" s="59"/>
       <c r="F7" s="38" t="s">
         <v>396</v>
       </c>
@@ -19921,10 +20044,10 @@
       <c r="C8" s="38">
         <v>3</v>
       </c>
-      <c r="D8" s="54">
+      <c r="D8" s="58">
         <v>7</v>
       </c>
-      <c r="E8" s="55"/>
+      <c r="E8" s="59"/>
       <c r="F8" s="38" t="s">
         <v>403</v>
       </c>
@@ -19936,9 +20059,9 @@
       <c r="B9" s="49" t="s">
         <v>431</v>
       </c>
-      <c r="C9" s="50"/>
-      <c r="D9" s="50"/>
-      <c r="E9" s="51"/>
+      <c r="C9" s="55"/>
+      <c r="D9" s="55"/>
+      <c r="E9" s="50"/>
       <c r="F9" s="40" t="s">
         <v>405</v>
       </c>
@@ -20010,7 +20133,7 @@
       <c r="D13" s="49">
         <v>23.6</v>
       </c>
-      <c r="E13" s="51"/>
+      <c r="E13" s="50"/>
       <c r="F13" s="38" t="s">
         <v>408</v>
       </c>
@@ -20023,8 +20146,8 @@
         <v>3.7000000000000002E-3</v>
       </c>
       <c r="C14" s="45"/>
-      <c r="D14" s="56"/>
-      <c r="E14" s="57"/>
+      <c r="D14" s="51"/>
+      <c r="E14" s="52"/>
       <c r="F14" s="40" t="s">
         <v>413</v>
       </c>
@@ -20042,7 +20165,7 @@
       <c r="D15" s="49" t="s">
         <v>417</v>
       </c>
-      <c r="E15" s="51"/>
+      <c r="E15" s="50"/>
       <c r="F15" s="38" t="s">
         <v>410</v>
       </c>
@@ -20060,7 +20183,7 @@
       <c r="D16" s="49" t="s">
         <v>421</v>
       </c>
-      <c r="E16" s="51"/>
+      <c r="E16" s="50"/>
       <c r="F16" s="38" t="s">
         <v>396</v>
       </c>
@@ -20075,27 +20198,27 @@
       <c r="C17" s="39" t="s">
         <v>424</v>
       </c>
-      <c r="D17" s="58" t="s">
+      <c r="D17" s="53" t="s">
         <v>425</v>
       </c>
-      <c r="E17" s="59"/>
+      <c r="E17" s="54"/>
       <c r="F17" s="40" t="s">
         <v>426</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="D17:E17"/>
     <mergeCell ref="B9:E9"/>
     <mergeCell ref="D4:E4"/>
     <mergeCell ref="D5:E5"/>
     <mergeCell ref="B6:E6"/>
     <mergeCell ref="D7:E7"/>
     <mergeCell ref="D8:E8"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="D17:E17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Fix error in deionized water dataset
</commit_message>
<xml_diff>
--- a/premise/data/additional_inventories/lci-hydrogen-electrolysis.xlsx
+++ b/premise/data/additional_inventories/lci-hydrogen-electrolysis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/romain/GitHub/premise/premise/data/additional_inventories/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57D8C29F-CA9A-4C42-A35D-878E671CD9FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3E1EBDD-60C2-3141-9321-53456E6339A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34920" yWindow="760" windowWidth="25800" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4440" yWindow="760" windowWidth="25800" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="lci" sheetId="1" r:id="rId1"/>
@@ -2221,22 +2221,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2250,6 +2238,18 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -2538,8 +2538,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U593"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A571" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B594" sqref="B594"/>
+    <sheetView tabSelected="1" topLeftCell="A558" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B590" sqref="B590"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -19403,8 +19403,8 @@
         <v>539</v>
       </c>
       <c r="B572" s="4">
-        <f>(5.2/0.000001)*(B571*1000)</f>
-        <v>2228571.4285714286</v>
+        <f>(5.2*0.000001)*(B571*1000)</f>
+        <v>2.2285714285714286E-6</v>
       </c>
       <c r="D572" t="s">
         <v>13</v>
@@ -19427,8 +19427,8 @@
         <v>541</v>
       </c>
       <c r="B573" s="4">
-        <f>(1.7/0.000001)*(B571*1000)</f>
-        <v>728571.42857142852</v>
+        <f>(1.7*0.000001)*(B571*1000)</f>
+        <v>7.2857142857142845E-7</v>
       </c>
       <c r="D573" t="s">
         <v>13</v>
@@ -19451,8 +19451,8 @@
         <v>543</v>
       </c>
       <c r="B574" s="4">
-        <f>(31/0.000001)*(B571*1000)</f>
-        <v>13285714.285714285</v>
+        <f>(31*0.000001)*(B571*1000)</f>
+        <v>1.3285714285714285E-5</v>
       </c>
       <c r="D574" t="s">
         <v>13</v>
@@ -19851,8 +19851,8 @@
         <v>539</v>
       </c>
       <c r="B591" s="4">
-        <f>(5.2/0.000001)*(B590*1000)</f>
-        <v>13000000</v>
+        <f>(5.2*0.000001)*(B590*1000)</f>
+        <v>1.3000000000000001E-5</v>
       </c>
       <c r="D591" t="s">
         <v>13</v>
@@ -19875,8 +19875,8 @@
         <v>541</v>
       </c>
       <c r="B592" s="4">
-        <f>(1.7/0.000001)*(B590*1000)</f>
-        <v>4250000</v>
+        <f>(1.7*0.000001)*(B590*1000)</f>
+        <v>4.25E-6</v>
       </c>
       <c r="D592" t="s">
         <v>13</v>
@@ -19899,8 +19899,8 @@
         <v>543</v>
       </c>
       <c r="B593" s="4">
-        <f>(31/0.000001)*(B590*1000)</f>
-        <v>77500000</v>
+        <f>(31*0.000001)*(B590*1000)</f>
+        <v>7.75E-5</v>
       </c>
       <c r="D593" t="s">
         <v>13</v>
@@ -19976,10 +19976,10 @@
       <c r="C4" s="38" t="s">
         <v>430</v>
       </c>
-      <c r="D4" s="56" t="s">
+      <c r="D4" s="52" t="s">
         <v>395</v>
       </c>
-      <c r="E4" s="57"/>
+      <c r="E4" s="53"/>
       <c r="F4" s="39" t="s">
         <v>396</v>
       </c>
@@ -19994,10 +19994,10 @@
       <c r="C5" s="38">
         <v>5.5</v>
       </c>
-      <c r="D5" s="58">
+      <c r="D5" s="54">
         <v>2.5</v>
       </c>
-      <c r="E5" s="59"/>
+      <c r="E5" s="55"/>
       <c r="F5" s="38" t="s">
         <v>397</v>
       </c>
@@ -20009,9 +20009,9 @@
       <c r="B6" s="49" t="s">
         <v>399</v>
       </c>
-      <c r="C6" s="55"/>
-      <c r="D6" s="55"/>
-      <c r="E6" s="50"/>
+      <c r="C6" s="50"/>
+      <c r="D6" s="50"/>
+      <c r="E6" s="51"/>
       <c r="F6" s="40" t="s">
         <v>400</v>
       </c>
@@ -20026,10 +20026,10 @@
       <c r="C7" s="38">
         <v>20</v>
       </c>
-      <c r="D7" s="58">
+      <c r="D7" s="54">
         <v>20</v>
       </c>
-      <c r="E7" s="59"/>
+      <c r="E7" s="55"/>
       <c r="F7" s="38" t="s">
         <v>396</v>
       </c>
@@ -20044,10 +20044,10 @@
       <c r="C8" s="38">
         <v>3</v>
       </c>
-      <c r="D8" s="58">
+      <c r="D8" s="54">
         <v>7</v>
       </c>
-      <c r="E8" s="59"/>
+      <c r="E8" s="55"/>
       <c r="F8" s="38" t="s">
         <v>403</v>
       </c>
@@ -20059,9 +20059,9 @@
       <c r="B9" s="49" t="s">
         <v>431</v>
       </c>
-      <c r="C9" s="55"/>
-      <c r="D9" s="55"/>
-      <c r="E9" s="50"/>
+      <c r="C9" s="50"/>
+      <c r="D9" s="50"/>
+      <c r="E9" s="51"/>
       <c r="F9" s="40" t="s">
         <v>405</v>
       </c>
@@ -20133,7 +20133,7 @@
       <c r="D13" s="49">
         <v>23.6</v>
       </c>
-      <c r="E13" s="50"/>
+      <c r="E13" s="51"/>
       <c r="F13" s="38" t="s">
         <v>408</v>
       </c>
@@ -20146,8 +20146,8 @@
         <v>3.7000000000000002E-3</v>
       </c>
       <c r="C14" s="45"/>
-      <c r="D14" s="51"/>
-      <c r="E14" s="52"/>
+      <c r="D14" s="56"/>
+      <c r="E14" s="57"/>
       <c r="F14" s="40" t="s">
         <v>413</v>
       </c>
@@ -20165,7 +20165,7 @@
       <c r="D15" s="49" t="s">
         <v>417</v>
       </c>
-      <c r="E15" s="50"/>
+      <c r="E15" s="51"/>
       <c r="F15" s="38" t="s">
         <v>410</v>
       </c>
@@ -20183,7 +20183,7 @@
       <c r="D16" s="49" t="s">
         <v>421</v>
       </c>
-      <c r="E16" s="50"/>
+      <c r="E16" s="51"/>
       <c r="F16" s="38" t="s">
         <v>396</v>
       </c>
@@ -20198,27 +20198,27 @@
       <c r="C17" s="39" t="s">
         <v>424</v>
       </c>
-      <c r="D17" s="53" t="s">
+      <c r="D17" s="58" t="s">
         <v>425</v>
       </c>
-      <c r="E17" s="54"/>
+      <c r="E17" s="59"/>
       <c r="F17" s="40" t="s">
         <v>426</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="D17:E17"/>
     <mergeCell ref="B9:E9"/>
     <mergeCell ref="D4:E4"/>
     <mergeCell ref="D5:E5"/>
     <mergeCell ref="B6:E6"/>
     <mergeCell ref="D7:E7"/>
     <mergeCell ref="D8:E8"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="D17:E17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>